<commit_message>
finished and tested path planning
</commit_message>
<xml_diff>
--- a/output files/TRC Heavy tank dia sweep files/sweep data.xlsx
+++ b/output files/TRC Heavy tank dia sweep files/sweep data.xlsx
@@ -535,22 +535,22 @@
         <v>1.23</v>
       </c>
       <c r="G2" t="n">
-        <v>3780518.414558016</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H2" t="n">
-        <v>107.6465219332719</v>
+        <v>64.11190241563072</v>
       </c>
       <c r="I2" t="n">
-        <v>3618475.846963029</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J2" t="n">
-        <v>162042.5675949869</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K2" t="n">
-        <v>0.0513</v>
+        <v>0.0461</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1606</v>
+        <v>0.101</v>
       </c>
       <c r="M2" t="n">
         <v>1500</v>
@@ -559,7 +559,7 @@
         <v>2000</v>
       </c>
       <c r="O2" t="n">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="P2" t="n">
         <v>1</v>
@@ -585,22 +585,22 @@
         <v>1.32</v>
       </c>
       <c r="G3" t="n">
-        <v>3780518.414558016</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H3" t="n">
-        <v>107.6465219332719</v>
+        <v>64.11190241563072</v>
       </c>
       <c r="I3" t="n">
-        <v>3618475.846963029</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J3" t="n">
-        <v>162042.5675949869</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K3" t="n">
-        <v>0.0513</v>
+        <v>0.0461</v>
       </c>
       <c r="L3" t="n">
-        <v>0.1606</v>
+        <v>0.101</v>
       </c>
       <c r="M3" t="n">
         <v>1500</v>
@@ -609,7 +609,7 @@
         <v>2000</v>
       </c>
       <c r="O3" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="P3" t="n">
         <v>1</v>
@@ -635,22 +635,22 @@
         <v>1.41</v>
       </c>
       <c r="G4" t="n">
-        <v>3847056.419182586</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H4" t="n">
-        <v>109.4686628467739</v>
+        <v>64.11190241563072</v>
       </c>
       <c r="I4" t="n">
-        <v>3698244.801962647</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J4" t="n">
-        <v>148811.6172199391</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K4" t="n">
-        <v>0.0488</v>
+        <v>0.0461</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1717</v>
+        <v>0.101</v>
       </c>
       <c r="M4" t="n">
         <v>1500</v>
@@ -659,7 +659,7 @@
         <v>2000</v>
       </c>
       <c r="O4" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="P4" t="n">
         <v>1</v>
@@ -685,22 +685,22 @@
         <v>1.23</v>
       </c>
       <c r="G5" t="n">
-        <v>4072815.181880503</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H5" t="n">
-        <v>108.4868264070309</v>
+        <v>61.28830538310085</v>
       </c>
       <c r="I5" t="n">
-        <v>3917556.118302241</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J5" t="n">
-        <v>155259.0635782623</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K5" t="n">
-        <v>0.05</v>
+        <v>0.0461</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1743</v>
+        <v>0.101</v>
       </c>
       <c r="M5" t="n">
         <v>1500</v>
@@ -709,7 +709,7 @@
         <v>2000</v>
       </c>
       <c r="O5" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="P5" t="n">
         <v>1</v>
@@ -735,22 +735,22 @@
         <v>1.32</v>
       </c>
       <c r="G6" t="n">
-        <v>4072815.181880503</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H6" t="n">
-        <v>108.4868264070309</v>
+        <v>61.28830538310085</v>
       </c>
       <c r="I6" t="n">
-        <v>3917556.118302241</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J6" t="n">
-        <v>155259.0635782623</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K6" t="n">
-        <v>0.05</v>
+        <v>0.0461</v>
       </c>
       <c r="L6" t="n">
-        <v>0.1743</v>
+        <v>0.101</v>
       </c>
       <c r="M6" t="n">
         <v>1500</v>
@@ -759,7 +759,7 @@
         <v>2000</v>
       </c>
       <c r="O6" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="P6" t="n">
         <v>1</v>
@@ -785,22 +785,22 @@
         <v>1.41</v>
       </c>
       <c r="G7" t="n">
-        <v>4163246.947544792</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H7" t="n">
-        <v>110.7222956744191</v>
+        <v>61.28830538310085</v>
       </c>
       <c r="I7" t="n">
-        <v>4020395.909941998</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J7" t="n">
-        <v>142851.0376027937</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0477</v>
+        <v>0.0461</v>
       </c>
       <c r="L7" t="n">
-        <v>0.1864</v>
+        <v>0.101</v>
       </c>
       <c r="M7" t="n">
         <v>1500</v>
@@ -809,7 +809,7 @@
         <v>2000</v>
       </c>
       <c r="O7" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="P7" t="n">
         <v>1</v>
@@ -835,22 +835,22 @@
         <v>1.23</v>
       </c>
       <c r="G8" t="n">
-        <v>4431780.797517795</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H8" t="n">
-        <v>110.469744949207</v>
+        <v>58.77510906724572</v>
       </c>
       <c r="I8" t="n">
-        <v>4283202.788682872</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J8" t="n">
-        <v>148578.0088349226</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K8" t="n">
-        <v>0.0487</v>
+        <v>0.0461</v>
       </c>
       <c r="L8" t="n">
-        <v>0.19</v>
+        <v>0.101</v>
       </c>
       <c r="M8" t="n">
         <v>1500</v>
@@ -859,7 +859,7 @@
         <v>2000</v>
       </c>
       <c r="O8" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="P8" t="n">
         <v>1</v>
@@ -885,22 +885,22 @@
         <v>1.32</v>
       </c>
       <c r="G9" t="n">
-        <v>4431780.797517795</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H9" t="n">
-        <v>110.469744949207</v>
+        <v>58.77510906724572</v>
       </c>
       <c r="I9" t="n">
-        <v>4283202.788682872</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J9" t="n">
-        <v>148578.0088349226</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0487</v>
+        <v>0.0461</v>
       </c>
       <c r="L9" t="n">
-        <v>0.19</v>
+        <v>0.101</v>
       </c>
       <c r="M9" t="n">
         <v>1500</v>
@@ -909,7 +909,7 @@
         <v>2000</v>
       </c>
       <c r="O9" t="n">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="P9" t="n">
         <v>1</v>
@@ -935,22 +935,22 @@
         <v>1.41</v>
       </c>
       <c r="G10" t="n">
-        <v>4571917.080040828</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H10" t="n">
-        <v>113.6218753732697</v>
+        <v>58.77510906724572</v>
       </c>
       <c r="I10" t="n">
-        <v>4436020.554591797</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J10" t="n">
-        <v>135896.5254490311</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0464</v>
+        <v>0.0461</v>
       </c>
       <c r="L10" t="n">
-        <v>0.2047</v>
+        <v>0.101</v>
       </c>
       <c r="M10" t="n">
         <v>1500</v>
@@ -959,7 +959,7 @@
         <v>2000</v>
       </c>
       <c r="O10" t="n">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="P10" t="n">
         <v>1</v>
@@ -985,22 +985,22 @@
         <v>1.23</v>
       </c>
       <c r="G11" t="n">
-        <v>4858843.426230708</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H11" t="n">
-        <v>113.3890095085117</v>
+        <v>56.53291518611289</v>
       </c>
       <c r="I11" t="n">
-        <v>4715715.237829252</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J11" t="n">
-        <v>143128.1884014556</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0476</v>
+        <v>0.0461</v>
       </c>
       <c r="L11" t="n">
-        <v>0.2065</v>
+        <v>0.101</v>
       </c>
       <c r="M11" t="n">
         <v>1500</v>
@@ -1009,7 +1009,7 @@
         <v>2000</v>
       </c>
       <c r="O11" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="P11" t="n">
         <v>1</v>
@@ -1035,22 +1035,22 @@
         <v>1.32</v>
       </c>
       <c r="G12" t="n">
-        <v>4858843.426230708</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H12" t="n">
-        <v>113.3890095085117</v>
+        <v>56.53291518611289</v>
       </c>
       <c r="I12" t="n">
-        <v>4715715.237829252</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J12" t="n">
-        <v>143128.1884014556</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K12" t="n">
-        <v>0.0476</v>
+        <v>0.0461</v>
       </c>
       <c r="L12" t="n">
-        <v>0.2065</v>
+        <v>0.101</v>
       </c>
       <c r="M12" t="n">
         <v>1500</v>
@@ -1059,7 +1059,7 @@
         <v>2000</v>
       </c>
       <c r="O12" t="n">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="P12" t="n">
         <v>1</v>
@@ -1085,22 +1085,22 @@
         <v>1.41</v>
       </c>
       <c r="G13" t="n">
-        <v>5104925.457941238</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H13" t="n">
-        <v>118.488522388827</v>
+        <v>56.53291518611289</v>
       </c>
       <c r="I13" t="n">
-        <v>4977055.204443134</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J13" t="n">
-        <v>127870.2534981033</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K13" t="n">
-        <v>0.0449</v>
+        <v>0.0461</v>
       </c>
       <c r="L13" t="n">
-        <v>0.2274</v>
+        <v>0.101</v>
       </c>
       <c r="M13" t="n">
         <v>1500</v>
@@ -1109,7 +1109,7 @@
         <v>2000</v>
       </c>
       <c r="O13" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="P13" t="n">
         <v>1</v>
@@ -1135,22 +1135,22 @@
         <v>1.23</v>
       </c>
       <c r="G14" t="n">
-        <v>5443828.498710256</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H14" t="n">
-        <v>118.7761231160407</v>
+        <v>54.5283836203006</v>
       </c>
       <c r="I14" t="n">
-        <v>5308213.520022186</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J14" t="n">
-        <v>135614.9786880709</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K14" t="n">
         <v>0.0461</v>
       </c>
       <c r="L14" t="n">
-        <v>0.2286</v>
+        <v>0.101</v>
       </c>
       <c r="M14" t="n">
         <v>1500</v>
@@ -1159,7 +1159,7 @@
         <v>2000</v>
       </c>
       <c r="O14" t="n">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="P14" t="n">
         <v>1</v>
@@ -1185,22 +1185,22 @@
         <v>1.32</v>
       </c>
       <c r="G15" t="n">
-        <v>5443828.498710256</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H15" t="n">
-        <v>118.7761231160407</v>
+        <v>54.5283836203006</v>
       </c>
       <c r="I15" t="n">
-        <v>5308213.520022186</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J15" t="n">
-        <v>135614.9786880709</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K15" t="n">
         <v>0.0461</v>
       </c>
       <c r="L15" t="n">
-        <v>0.2286</v>
+        <v>0.101</v>
       </c>
       <c r="M15" t="n">
         <v>1500</v>
@@ -1209,7 +1209,7 @@
         <v>2000</v>
       </c>
       <c r="O15" t="n">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="P15" t="n">
         <v>1</v>
@@ -1235,22 +1235,22 @@
         <v>1.41</v>
       </c>
       <c r="G16" t="n">
-        <v>5754564.868966291</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H16" t="n">
-        <v>124.753138226594</v>
+        <v>54.5283836203006</v>
       </c>
       <c r="I16" t="n">
-        <v>5632327.813187371</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J16" t="n">
-        <v>122237.0557789197</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K16" t="n">
-        <v>0.0438</v>
+        <v>0.0461</v>
       </c>
       <c r="L16" t="n">
-        <v>0.2501</v>
+        <v>0.101</v>
       </c>
       <c r="M16" t="n">
         <v>1500</v>
@@ -1259,7 +1259,7 @@
         <v>2000</v>
       </c>
       <c r="O16" t="n">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="P16" t="n">
         <v>1</v>
@@ -1285,22 +1285,22 @@
         <v>1.23</v>
       </c>
       <c r="G17" t="n">
-        <v>6157802.997946491</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H17" t="n">
-        <v>125.6232566370581</v>
+        <v>52.73314798945927</v>
       </c>
       <c r="I17" t="n">
-        <v>6027842.569096862</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J17" t="n">
-        <v>129960.4288496292</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K17" t="n">
-        <v>0.0449</v>
+        <v>0.0461</v>
       </c>
       <c r="L17" t="n">
-        <v>0.2512</v>
+        <v>0.101</v>
       </c>
       <c r="M17" t="n">
         <v>1500</v>
@@ -1309,7 +1309,7 @@
         <v>2000</v>
       </c>
       <c r="O17" t="n">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="P17" t="n">
         <v>1</v>
@@ -1335,22 +1335,22 @@
         <v>1.32</v>
       </c>
       <c r="G18" t="n">
-        <v>6157802.997946491</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H18" t="n">
-        <v>125.6232566370581</v>
+        <v>52.73314798945927</v>
       </c>
       <c r="I18" t="n">
-        <v>6027842.569096862</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J18" t="n">
-        <v>129960.4288496292</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K18" t="n">
-        <v>0.0449</v>
+        <v>0.0461</v>
       </c>
       <c r="L18" t="n">
-        <v>0.2512</v>
+        <v>0.101</v>
       </c>
       <c r="M18" t="n">
         <v>1500</v>
@@ -1359,7 +1359,7 @@
         <v>2000</v>
       </c>
       <c r="O18" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="P18" t="n">
         <v>1</v>
@@ -1385,22 +1385,22 @@
         <v>1.41</v>
       </c>
       <c r="G19" t="n">
-        <v>6579644.563832727</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H19" t="n">
-        <v>133.2039618423134</v>
+        <v>52.73314798945927</v>
       </c>
       <c r="I19" t="n">
-        <v>6462924.76463033</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J19" t="n">
-        <v>116719.7992023974</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0427</v>
+        <v>0.0461</v>
       </c>
       <c r="L19" t="n">
-        <v>0.2754</v>
+        <v>0.101</v>
       </c>
       <c r="M19" t="n">
         <v>1500</v>
@@ -1409,7 +1409,7 @@
         <v>2000</v>
       </c>
       <c r="O19" t="n">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="P19" t="n">
         <v>1</v>
@@ -1435,22 +1435,22 @@
         <v>1.23</v>
       </c>
       <c r="G20" t="n">
-        <v>7018964.403628038</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H20" t="n">
-        <v>133.9958164102094</v>
+        <v>51.12295111925128</v>
       </c>
       <c r="I20" t="n">
-        <v>6895299.718880384</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J20" t="n">
-        <v>123664.6847476543</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0436</v>
+        <v>0.0461</v>
       </c>
       <c r="L20" t="n">
-        <v>0.2763</v>
+        <v>0.101</v>
       </c>
       <c r="M20" t="n">
         <v>1500</v>
@@ -1459,7 +1459,7 @@
         <v>2000</v>
       </c>
       <c r="O20" t="n">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="P20" t="n">
         <v>1</v>
@@ -1485,22 +1485,22 @@
         <v>1.32</v>
       </c>
       <c r="G21" t="n">
-        <v>7018964.403628038</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H21" t="n">
-        <v>133.9958164102094</v>
+        <v>51.12295111925128</v>
       </c>
       <c r="I21" t="n">
-        <v>6895299.718880384</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J21" t="n">
-        <v>123664.6847476543</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K21" t="n">
-        <v>0.0436</v>
+        <v>0.0461</v>
       </c>
       <c r="L21" t="n">
-        <v>0.2763</v>
+        <v>0.101</v>
       </c>
       <c r="M21" t="n">
         <v>1500</v>
@@ -1509,7 +1509,7 @@
         <v>2000</v>
       </c>
       <c r="O21" t="n">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="P21" t="n">
         <v>1</v>
@@ -1535,22 +1535,22 @@
         <v>1.41</v>
       </c>
       <c r="G22" t="n">
-        <v>7825811.998415833</v>
+        <v>1458377.232148911</v>
       </c>
       <c r="H22" t="n">
-        <v>147.4946619139004</v>
+        <v>51.12295111925128</v>
       </c>
       <c r="I22" t="n">
-        <v>7715639.964505017</v>
+        <v>1344745.458720702</v>
       </c>
       <c r="J22" t="n">
-        <v>110172.0339108169</v>
+        <v>113631.7734282086</v>
       </c>
       <c r="K22" t="n">
-        <v>0.0414</v>
+        <v>0.0461</v>
       </c>
       <c r="L22" t="n">
-        <v>0.3081</v>
+        <v>0.101</v>
       </c>
       <c r="M22" t="n">
         <v>1500</v>
@@ -1559,7 +1559,7 @@
         <v>2000</v>
       </c>
       <c r="O22" t="n">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="P22" t="n">
         <v>1</v>

</xml_diff>